<commit_message>
New Home Page Layout
</commit_message>
<xml_diff>
--- a/Tkinter Stuff/Spot_TD Layout.xlsx
+++ b/Tkinter Stuff/Spot_TD Layout.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\spot_td\Tkinter Stuff\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1C8EAB6A-B466-42C0-B1AC-6EF5A816BCDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C2B6D03-0E0B-4A36-A71A-FDFFA5F1A693}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{ADCF53F3-C3B1-4CE8-B7B4-70BC1F439B47}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{ADCF53F3-C3B1-4CE8-B7B4-70BC1F439B47}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,18 +36,66 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="20">
   <si>
     <t>Landing Page</t>
   </si>
   <si>
-    <t>Main Menu</t>
-  </si>
-  <si>
     <t>Connections</t>
   </si>
   <si>
     <t>Connected (Show Name) / Not Connected (Find Connection / Disconnect)</t>
+  </si>
+  <si>
+    <t>Home Page</t>
+  </si>
+  <si>
+    <t>Kill Button</t>
+  </si>
+  <si>
+    <t>Nav</t>
+  </si>
+  <si>
+    <t>Label</t>
+  </si>
+  <si>
+    <t>Home Frame</t>
+  </si>
+  <si>
+    <t>Menu frame</t>
+  </si>
+  <si>
+    <t>Connections frame</t>
+  </si>
+  <si>
+    <t>Connection button</t>
+  </si>
+  <si>
+    <t>Connections status window</t>
+  </si>
+  <si>
+    <t>Nav frame</t>
+  </si>
+  <si>
+    <t>Nav button</t>
+  </si>
+  <si>
+    <t>Nav status window</t>
+  </si>
+  <si>
+    <t>Settings frame</t>
+  </si>
+  <si>
+    <t>Settings button</t>
+  </si>
+  <si>
+    <t>Settings status window</t>
+  </si>
+  <si>
+    <t>(remove in final)</t>
+  </si>
+  <si>
+    <t>Settings</t>
   </si>
 </sst>
 </file>
@@ -207,13 +255,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
@@ -227,7 +274,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -258,6 +304,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -572,21 +619,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99CA2281-E782-4E98-989A-66F3E0F43DB4}">
-  <dimension ref="A1:K30"/>
+  <dimension ref="A1:P30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="3" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="M2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="1"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
@@ -598,33 +649,36 @@
       <c r="J3" s="2"/>
       <c r="K3" s="3"/>
     </row>
-    <row r="4" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="4"/>
-      <c r="C4" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="D4" s="11"/>
-      <c r="E4" s="11"/>
-      <c r="F4" s="11"/>
-      <c r="G4" s="11"/>
-      <c r="H4" s="11"/>
-      <c r="I4" s="11"/>
-      <c r="J4" s="12"/>
-      <c r="K4" s="6"/>
-    </row>
-    <row r="5" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C4" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="10"/>
+      <c r="H4" s="10"/>
+      <c r="I4" s="10"/>
+      <c r="J4" s="11"/>
+      <c r="K4" s="5"/>
+      <c r="N4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="4"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
-      <c r="H5" s="5"/>
-      <c r="I5" s="5"/>
-      <c r="J5" s="5"/>
-      <c r="K5" s="6"/>
-    </row>
-    <row r="6" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C5" s="22"/>
+      <c r="D5" s="22"/>
+      <c r="E5" s="22"/>
+      <c r="F5" s="22"/>
+      <c r="G5" s="22"/>
+      <c r="H5" s="22"/>
+      <c r="I5" s="22"/>
+      <c r="J5" s="22"/>
+      <c r="K5" s="5"/>
+    </row>
+    <row r="6" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="4"/>
       <c r="C6" s="1"/>
       <c r="D6" s="2"/>
@@ -634,305 +688,348 @@
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
       <c r="J6" s="3"/>
-      <c r="K6" s="6"/>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K6" s="5"/>
+      <c r="N6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
-      <c r="D7" s="14" t="s">
+      <c r="D7" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="E7" s="13"/>
+      <c r="F7" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="E7" s="15"/>
-      <c r="F7" s="18" t="s">
-        <v>3</v>
-      </c>
-      <c r="G7" s="19"/>
-      <c r="H7" s="19"/>
-      <c r="I7" s="20"/>
-      <c r="J7" s="6"/>
-      <c r="K7" s="6"/>
-    </row>
-    <row r="8" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G7" s="17"/>
+      <c r="H7" s="17"/>
+      <c r="I7" s="18"/>
+      <c r="J7" s="5"/>
+      <c r="K7" s="5"/>
+      <c r="O7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
-      <c r="D8" s="16"/>
-      <c r="E8" s="17"/>
-      <c r="F8" s="21"/>
-      <c r="G8" s="22"/>
-      <c r="H8" s="22"/>
-      <c r="I8" s="23"/>
-      <c r="J8" s="6"/>
-      <c r="K8" s="6"/>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="D8" s="14"/>
+      <c r="E8" s="15"/>
+      <c r="F8" s="19"/>
+      <c r="G8" s="20"/>
+      <c r="H8" s="20"/>
+      <c r="I8" s="21"/>
+      <c r="J8" s="5"/>
+      <c r="K8" s="5"/>
+      <c r="P8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="5"/>
-      <c r="H9" s="5"/>
-      <c r="I9" s="5"/>
-      <c r="J9" s="6"/>
-      <c r="K9" s="6"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="D9" s="22"/>
+      <c r="E9" s="22"/>
+      <c r="F9" s="22"/>
+      <c r="G9" s="22"/>
+      <c r="H9" s="22"/>
+      <c r="I9" s="22"/>
+      <c r="J9" s="5"/>
+      <c r="K9" s="5"/>
+      <c r="P9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="5"/>
-      <c r="H10" s="13"/>
-      <c r="I10" s="5"/>
-      <c r="J10" s="6"/>
-      <c r="K10" s="6"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="D10" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="E10" s="13"/>
+      <c r="F10" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="G10" s="17"/>
+      <c r="H10" s="17"/>
+      <c r="I10" s="18"/>
+      <c r="J10" s="5"/>
+      <c r="K10" s="5"/>
+      <c r="O10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
-      <c r="G11" s="5"/>
-      <c r="H11" s="5"/>
-      <c r="I11" s="5"/>
-      <c r="J11" s="6"/>
-      <c r="K11" s="6"/>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="D11" s="14"/>
+      <c r="E11" s="15"/>
+      <c r="F11" s="19"/>
+      <c r="G11" s="20"/>
+      <c r="H11" s="20"/>
+      <c r="I11" s="21"/>
+      <c r="J11" s="5"/>
+      <c r="K11" s="5"/>
+      <c r="P11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="5"/>
-      <c r="H12" s="5"/>
-      <c r="I12" s="5"/>
-      <c r="J12" s="6"/>
-      <c r="K12" s="6"/>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="D12" s="22"/>
+      <c r="E12" s="22"/>
+      <c r="F12" s="22"/>
+      <c r="G12" s="22"/>
+      <c r="H12" s="22"/>
+      <c r="I12" s="22"/>
+      <c r="J12" s="5"/>
+      <c r="K12" s="5"/>
+      <c r="P12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="5"/>
-      <c r="G13" s="5"/>
-      <c r="H13" s="5"/>
-      <c r="I13" s="5"/>
-      <c r="J13" s="6"/>
-      <c r="K13" s="6"/>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="D13" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="E13" s="13"/>
+      <c r="F13" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="G13" s="17"/>
+      <c r="H13" s="17"/>
+      <c r="I13" s="18"/>
+      <c r="J13" s="5"/>
+      <c r="K13" s="5"/>
+      <c r="O13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="5"/>
-      <c r="H14" s="5"/>
-      <c r="I14" s="5"/>
-      <c r="J14" s="6"/>
-      <c r="K14" s="6"/>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="D14" s="14"/>
+      <c r="E14" s="15"/>
+      <c r="F14" s="19"/>
+      <c r="G14" s="20"/>
+      <c r="H14" s="20"/>
+      <c r="I14" s="21"/>
+      <c r="J14" s="5"/>
+      <c r="K14" s="5"/>
+      <c r="P14" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
-      <c r="F15" s="5"/>
-      <c r="G15" s="5"/>
-      <c r="H15" s="5"/>
-      <c r="I15" s="5"/>
-      <c r="J15" s="6"/>
-      <c r="K15" s="6"/>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="D15" s="22"/>
+      <c r="E15" s="22"/>
+      <c r="F15" s="22"/>
+      <c r="G15" s="22"/>
+      <c r="H15" s="22"/>
+      <c r="I15" s="22"/>
+      <c r="J15" s="5"/>
+      <c r="K15" s="5"/>
+      <c r="P15" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B16" s="4"/>
-      <c r="C16" s="4"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
-      <c r="F16" s="5"/>
-      <c r="G16" s="5"/>
-      <c r="H16" s="5"/>
-      <c r="I16" s="5"/>
-      <c r="J16" s="6"/>
-      <c r="K16" s="6"/>
-    </row>
-    <row r="17" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="C16" s="6"/>
+      <c r="D16" s="7"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="7"/>
+      <c r="G16" s="7"/>
+      <c r="H16" s="7"/>
+      <c r="I16" s="7"/>
+      <c r="J16" s="8"/>
+      <c r="K16" s="5"/>
+    </row>
+    <row r="17" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="4"/>
-      <c r="C17" s="4"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5"/>
-      <c r="F17" s="5"/>
-      <c r="G17" s="5"/>
-      <c r="H17" s="5"/>
-      <c r="I17" s="5"/>
-      <c r="J17" s="6"/>
-      <c r="K17" s="6"/>
-    </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="C17" s="22"/>
+      <c r="D17" s="22"/>
+      <c r="E17" s="22"/>
+      <c r="F17" s="22"/>
+      <c r="G17" s="22"/>
+      <c r="H17" s="22"/>
+      <c r="I17" s="22"/>
+      <c r="J17" s="22"/>
+      <c r="K17" s="5"/>
+    </row>
+    <row r="18" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B18" s="4"/>
-      <c r="C18" s="4"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
-      <c r="F18" s="5"/>
-      <c r="G18" s="5"/>
-      <c r="H18" s="5"/>
-      <c r="I18" s="5"/>
-      <c r="J18" s="6"/>
-      <c r="K18" s="6"/>
-    </row>
-    <row r="19" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B19" s="4"/>
-      <c r="C19" s="4"/>
-      <c r="D19" s="5"/>
-      <c r="E19" s="5"/>
-      <c r="F19" s="5"/>
-      <c r="G19" s="5"/>
-      <c r="H19" s="5"/>
-      <c r="I19" s="5"/>
-      <c r="J19" s="6"/>
-      <c r="K19" s="6"/>
-    </row>
-    <row r="20" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B20" s="4"/>
-      <c r="C20" s="4"/>
-      <c r="D20" s="5"/>
-      <c r="E20" s="5"/>
-      <c r="F20" s="5"/>
-      <c r="G20" s="5"/>
-      <c r="H20" s="5"/>
-      <c r="I20" s="5"/>
-      <c r="J20" s="6"/>
-      <c r="K20" s="6"/>
-    </row>
-    <row r="21" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B21" s="4"/>
-      <c r="C21" s="4"/>
-      <c r="D21" s="5"/>
-      <c r="E21" s="5"/>
-      <c r="F21" s="5"/>
-      <c r="G21" s="5"/>
-      <c r="H21" s="5"/>
-      <c r="I21" s="5"/>
-      <c r="J21" s="6"/>
-      <c r="K21" s="6"/>
-    </row>
-    <row r="22" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B22" s="4"/>
-      <c r="C22" s="4"/>
-      <c r="D22" s="5"/>
-      <c r="E22" s="5"/>
-      <c r="F22" s="5"/>
-      <c r="G22" s="5"/>
-      <c r="H22" s="5"/>
-      <c r="I22" s="5"/>
-      <c r="J22" s="6"/>
-      <c r="K22" s="6"/>
-    </row>
-    <row r="23" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B23" s="4"/>
-      <c r="C23" s="4"/>
-      <c r="D23" s="5"/>
-      <c r="E23" s="5"/>
-      <c r="F23" s="5"/>
-      <c r="G23" s="5"/>
-      <c r="H23" s="5"/>
-      <c r="I23" s="5"/>
-      <c r="J23" s="6"/>
-      <c r="K23" s="6"/>
-    </row>
-    <row r="24" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B24" s="4"/>
-      <c r="C24" s="4"/>
-      <c r="D24" s="5"/>
-      <c r="E24" s="5"/>
-      <c r="F24" s="5"/>
-      <c r="G24" s="5"/>
-      <c r="H24" s="5"/>
-      <c r="I24" s="5"/>
-      <c r="J24" s="6"/>
-      <c r="K24" s="6"/>
-    </row>
-    <row r="25" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B25" s="4"/>
-      <c r="C25" s="4"/>
-      <c r="D25" s="5"/>
-      <c r="E25" s="5"/>
-      <c r="F25" s="5"/>
-      <c r="G25" s="5"/>
-      <c r="H25" s="5"/>
-      <c r="I25" s="5"/>
-      <c r="J25" s="6"/>
-      <c r="K25" s="6"/>
-    </row>
-    <row r="26" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B26" s="4"/>
-      <c r="C26" s="4"/>
-      <c r="D26" s="5"/>
-      <c r="E26" s="5"/>
-      <c r="F26" s="5"/>
-      <c r="G26" s="5"/>
-      <c r="H26" s="5"/>
-      <c r="I26" s="5"/>
-      <c r="J26" s="6"/>
-      <c r="K26" s="6"/>
-    </row>
-    <row r="27" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B27" s="4"/>
-      <c r="C27" s="4"/>
-      <c r="D27" s="5"/>
-      <c r="E27" s="5"/>
-      <c r="F27" s="5"/>
-      <c r="G27" s="5"/>
-      <c r="H27" s="5"/>
-      <c r="I27" s="5"/>
-      <c r="J27" s="6"/>
-      <c r="K27" s="6"/>
-    </row>
-    <row r="28" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B28" s="4"/>
-      <c r="C28" s="4"/>
-      <c r="D28" s="5"/>
-      <c r="E28" s="5"/>
-      <c r="F28" s="5"/>
-      <c r="G28" s="5"/>
-      <c r="H28" s="5"/>
-      <c r="I28" s="5"/>
-      <c r="J28" s="6"/>
-      <c r="K28" s="6"/>
-    </row>
-    <row r="29" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B29" s="4"/>
-      <c r="C29" s="7"/>
-      <c r="D29" s="8"/>
-      <c r="E29" s="8"/>
-      <c r="F29" s="8"/>
-      <c r="G29" s="8"/>
-      <c r="H29" s="8"/>
-      <c r="I29" s="8"/>
-      <c r="J29" s="9"/>
-      <c r="K29" s="6"/>
-    </row>
-    <row r="30" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B30" s="7"/>
-      <c r="C30" s="8"/>
-      <c r="D30" s="8"/>
-      <c r="E30" s="8"/>
-      <c r="F30" s="8"/>
-      <c r="G30" s="8"/>
-      <c r="H30" s="8"/>
-      <c r="I30" s="8"/>
-      <c r="J30" s="8"/>
-      <c r="K30" s="9"/>
+      <c r="C18" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D18" s="10"/>
+      <c r="E18" s="10"/>
+      <c r="F18" s="10"/>
+      <c r="G18" s="10"/>
+      <c r="H18" s="10"/>
+      <c r="I18" s="10"/>
+      <c r="J18" s="11"/>
+      <c r="K18" s="5"/>
+      <c r="N18" t="s">
+        <v>4</v>
+      </c>
+      <c r="O18" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="6"/>
+      <c r="C19" s="7"/>
+      <c r="D19" s="7"/>
+      <c r="E19" s="7"/>
+      <c r="F19" s="7"/>
+      <c r="G19" s="7"/>
+      <c r="H19" s="7"/>
+      <c r="I19" s="7"/>
+      <c r="J19" s="7"/>
+      <c r="K19" s="8"/>
+    </row>
+    <row r="20" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B20" s="22"/>
+      <c r="C20" s="22"/>
+      <c r="D20" s="22"/>
+      <c r="E20" s="22"/>
+      <c r="F20" s="22"/>
+      <c r="G20" s="22"/>
+      <c r="H20" s="22"/>
+      <c r="I20" s="22"/>
+      <c r="J20" s="22"/>
+      <c r="K20" s="22"/>
+    </row>
+    <row r="21" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B21" s="22"/>
+      <c r="C21" s="22"/>
+      <c r="D21" s="22"/>
+      <c r="E21" s="22"/>
+      <c r="F21" s="22"/>
+      <c r="G21" s="22"/>
+      <c r="H21" s="22"/>
+      <c r="I21" s="22"/>
+      <c r="J21" s="22"/>
+      <c r="K21" s="22"/>
+    </row>
+    <row r="22" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B22" s="22"/>
+      <c r="C22" s="22"/>
+      <c r="D22" s="22"/>
+      <c r="E22" s="22"/>
+      <c r="F22" s="22"/>
+      <c r="G22" s="22"/>
+      <c r="H22" s="22"/>
+      <c r="I22" s="22"/>
+      <c r="J22" s="22"/>
+      <c r="K22" s="22"/>
+    </row>
+    <row r="23" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B23" s="22"/>
+      <c r="C23" s="22"/>
+      <c r="D23" s="22"/>
+      <c r="E23" s="22"/>
+      <c r="F23" s="22"/>
+      <c r="G23" s="22"/>
+      <c r="H23" s="22"/>
+      <c r="I23" s="22"/>
+      <c r="J23" s="22"/>
+      <c r="K23" s="22"/>
+    </row>
+    <row r="24" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B24" s="22"/>
+      <c r="C24" s="22"/>
+      <c r="D24" s="22"/>
+      <c r="E24" s="22"/>
+      <c r="F24" s="22"/>
+      <c r="G24" s="22"/>
+      <c r="H24" s="22"/>
+      <c r="I24" s="22"/>
+      <c r="J24" s="22"/>
+      <c r="K24" s="22"/>
+    </row>
+    <row r="25" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B25" s="22"/>
+      <c r="C25" s="22"/>
+      <c r="D25" s="22"/>
+      <c r="E25" s="22"/>
+      <c r="F25" s="22"/>
+      <c r="G25" s="22"/>
+      <c r="H25" s="22"/>
+      <c r="I25" s="22"/>
+      <c r="J25" s="22"/>
+      <c r="K25" s="22"/>
+    </row>
+    <row r="26" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B26" s="22"/>
+      <c r="C26" s="22"/>
+      <c r="D26" s="22"/>
+      <c r="E26" s="22"/>
+      <c r="F26" s="22"/>
+      <c r="G26" s="22"/>
+      <c r="H26" s="22"/>
+      <c r="I26" s="22"/>
+      <c r="J26" s="22"/>
+      <c r="K26" s="22"/>
+    </row>
+    <row r="27" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B27" s="22"/>
+      <c r="C27" s="22"/>
+      <c r="D27" s="22"/>
+      <c r="E27" s="22"/>
+      <c r="F27" s="22"/>
+      <c r="G27" s="22"/>
+      <c r="H27" s="22"/>
+      <c r="I27" s="22"/>
+      <c r="J27" s="22"/>
+      <c r="K27" s="22"/>
+    </row>
+    <row r="28" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B28" s="22"/>
+      <c r="C28" s="22"/>
+      <c r="D28" s="22"/>
+      <c r="E28" s="22"/>
+      <c r="F28" s="22"/>
+      <c r="G28" s="22"/>
+      <c r="H28" s="22"/>
+      <c r="I28" s="22"/>
+      <c r="J28" s="22"/>
+      <c r="K28" s="22"/>
+    </row>
+    <row r="29" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B29" s="22"/>
+      <c r="K29" s="22"/>
+    </row>
+    <row r="30" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B30" s="22"/>
+      <c r="C30" s="22"/>
+      <c r="D30" s="22"/>
+      <c r="E30" s="22"/>
+      <c r="F30" s="22"/>
+      <c r="G30" s="22"/>
+      <c r="H30" s="22"/>
+      <c r="I30" s="22"/>
+      <c r="J30" s="22"/>
+      <c r="K30" s="22"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="8">
+    <mergeCell ref="C18:J18"/>
+    <mergeCell ref="D13:E14"/>
+    <mergeCell ref="F13:I14"/>
     <mergeCell ref="C4:J4"/>
     <mergeCell ref="D7:E8"/>
     <mergeCell ref="F7:I8"/>
+    <mergeCell ref="D10:E11"/>
+    <mergeCell ref="F10:I11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>